<commit_message>
financial soundness indicators update
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukraine_data\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukrainedb\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5489FF9A-9786-44A1-AA37-05DD876DFA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2304C698-0D25-43DE-916A-0AC4D829E297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="367">
   <si>
     <t>source</t>
   </si>
@@ -220,9 +220,6 @@
     <t>interest_rates</t>
   </si>
   <si>
-    <t>https://bank.gov.ua/files/fsi_table_1_e.xlsx</t>
-  </si>
-  <si>
     <t>financial_soundness</t>
   </si>
   <si>
@@ -1154,6 +1151,12 @@
   </si>
   <si>
     <t>https://data.humdata.org/dataset/0d36e8ad-d2e8-4646-babd-61a41f99159a/resource/b6f75de1-4b73-4870-9c30-0e3d1c919e76/download_metadata?format=csv</t>
+  </si>
+  <si>
+    <t>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</t>
+  </si>
+  <si>
+    <t>FSIs SDDS Plus</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1574,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1604,7 +1607,7 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1618,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1641,7 +1644,7 @@
         <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1681,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1902,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>44</v>
@@ -1925,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>44</v>
@@ -1948,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>44</v>
@@ -2063,16 +2066,19 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>54</v>
+        <v>365</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>366</v>
       </c>
       <c r="H22">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2086,10 +2092,10 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -2109,10 +2115,10 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -2132,10 +2138,10 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -2155,11 +2161,10 @@
     <hyperlink ref="E25" r:id="rId7" xr:uid="{04E46315-FB46-4EB7-B7CC-4D046B83538C}"/>
     <hyperlink ref="E24" r:id="rId8" xr:uid="{66BBB48B-BFE8-486A-9602-D62D27CCB40F}"/>
     <hyperlink ref="E23" r:id="rId9" xr:uid="{373411FC-DB71-4A1B-8AF1-FD47374CEAD6}"/>
-    <hyperlink ref="E22" r:id="rId10" xr:uid="{864CD154-F73E-4563-B7B3-4902C4F5B214}"/>
-    <hyperlink ref="E20" r:id="rId11" xr:uid="{A0042D51-75FF-4622-92B3-F85244BF1565}"/>
-    <hyperlink ref="E21" r:id="rId12" xr:uid="{34D6EFF7-F5DE-4487-A837-7043BEBA7731}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{CB2ABF31-9EE8-4678-BF7F-C2E399CDD67F}"/>
-    <hyperlink ref="E3" r:id="rId14" xr:uid="{8E9E6E0C-1C15-4692-9DB7-C338EBCC85EF}"/>
+    <hyperlink ref="E20" r:id="rId10" xr:uid="{A0042D51-75FF-4622-92B3-F85244BF1565}"/>
+    <hyperlink ref="E21" r:id="rId11" xr:uid="{34D6EFF7-F5DE-4487-A837-7043BEBA7731}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{CB2ABF31-9EE8-4678-BF7F-C2E399CDD67F}"/>
+    <hyperlink ref="E3" r:id="rId13" xr:uid="{8E9E6E0C-1C15-4692-9DB7-C338EBCC85EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2181,7 +2186,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -2189,7 +2194,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2197,7 +2202,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2205,7 +2210,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2213,7 +2218,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2221,7 +2226,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2229,7 +2234,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2237,7 +2242,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2245,7 +2250,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2253,7 +2258,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2261,7 +2266,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2291,57 +2296,57 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>222</v>
-      </c>
-      <c r="C2" t="s">
-        <v>223</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2355,13 +2360,13 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
         <v>224</v>
       </c>
-      <c r="B3" t="s">
-        <v>225</v>
-      </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2375,13 +2380,13 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2395,13 +2400,13 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2415,13 +2420,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
         <v>228</v>
       </c>
-      <c r="B6" t="s">
-        <v>229</v>
-      </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2435,13 +2440,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2455,13 +2460,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2475,13 +2480,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2495,13 +2500,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2515,13 +2520,13 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2535,13 +2540,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2555,13 +2560,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2575,13 +2580,13 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2595,13 +2600,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2615,13 +2620,13 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2635,13 +2640,13 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2655,13 +2660,13 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2675,13 +2680,13 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2695,13 +2700,13 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2715,13 +2720,13 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2735,13 +2740,13 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2755,13 +2760,13 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" t="s">
         <v>222</v>
-      </c>
-      <c r="C23" t="s">
-        <v>223</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2775,13 +2780,13 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2790,22 +2795,22 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N24" t="str">
         <f>+sources!E20</f>
@@ -2814,13 +2819,13 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2829,22 +2834,22 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>284</v>
+      </c>
+      <c r="G25" t="s">
         <v>285</v>
       </c>
-      <c r="G25" t="s">
-        <v>286</v>
-      </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N25" t="str">
         <f>+sources!E18</f>
@@ -2853,13 +2858,13 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2868,16 +2873,16 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>284</v>
+      </c>
+      <c r="G26" t="s">
         <v>285</v>
       </c>
-      <c r="G26" t="s">
-        <v>286</v>
-      </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N26" t="str">
         <f>+sources!E18</f>
@@ -2886,13 +2891,13 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2904,21 +2909,21 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2927,33 +2932,33 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
+        <v>287</v>
+      </c>
+      <c r="G28" t="s">
         <v>288</v>
       </c>
-      <c r="G28" t="s">
-        <v>289</v>
-      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2962,33 +2967,33 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2997,39 +3002,39 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J30" t="s">
+        <v>344</v>
+      </c>
+      <c r="K30" t="s">
         <v>345</v>
       </c>
-      <c r="K30" t="s">
-        <v>346</v>
-      </c>
       <c r="M30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3038,39 +3043,39 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3079,34 +3084,34 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N32" t="str">
         <f>+sources!E22</f>
-        <v>https://bank.gov.ua/files/fsi_table_1_e.xlsx</v>
+        <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3115,19 +3120,19 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N33" t="str">
         <f>+sources!E23</f>
@@ -3136,13 +3141,13 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3151,22 +3156,22 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N34" t="str">
         <f>+sources!E15</f>
@@ -3175,13 +3180,13 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3190,25 +3195,25 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
+        <v>339</v>
+      </c>
+      <c r="J35" t="s">
         <v>340</v>
       </c>
-      <c r="J35" t="s">
-        <v>341</v>
-      </c>
       <c r="K35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N35" t="str">
         <f>+sources!E16</f>
@@ -3217,13 +3222,13 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -3232,22 +3237,22 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N36" t="str">
         <f>+sources!E15</f>
@@ -3256,13 +3261,13 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3271,30 +3276,30 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
+        <v>293</v>
+      </c>
+      <c r="G37" t="s">
         <v>294</v>
       </c>
-      <c r="G37" t="s">
-        <v>295</v>
-      </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3303,28 +3308,28 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
+        <v>352</v>
+      </c>
+      <c r="G38" t="s">
+        <v>295</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>321</v>
+      </c>
+      <c r="J38" t="s">
+        <v>355</v>
+      </c>
+      <c r="K38" t="s">
+        <v>354</v>
+      </c>
+      <c r="L38" t="s">
         <v>353</v>
       </c>
-      <c r="G38" t="s">
-        <v>296</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>322</v>
-      </c>
-      <c r="J38" t="s">
-        <v>356</v>
-      </c>
-      <c r="K38" t="s">
-        <v>355</v>
-      </c>
-      <c r="L38" t="s">
-        <v>354</v>
-      </c>
       <c r="M38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N38" t="e">
         <f>+sources!#REF!</f>
@@ -3333,13 +3338,13 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -3348,19 +3353,19 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
+        <v>306</v>
+      </c>
+      <c r="G39" t="s">
         <v>307</v>
       </c>
-      <c r="G39" t="s">
-        <v>308</v>
-      </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N39" t="e">
         <f>+sources!#REF!</f>
@@ -3369,13 +3374,13 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -3384,19 +3389,19 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N40" t="str">
         <f>+sources!E2</f>
@@ -3405,13 +3410,13 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3420,19 +3425,19 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G41" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N41" t="str">
         <f>+sources!E2</f>
@@ -3441,13 +3446,13 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3456,19 +3461,19 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N42" t="str">
         <f>+sources!E2</f>
@@ -3477,13 +3482,13 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3492,19 +3497,19 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N43" t="str">
         <f>+sources!E2</f>
@@ -3513,13 +3518,13 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B44" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3528,28 +3533,28 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
+        <v>327</v>
+      </c>
+      <c r="G44" t="s">
         <v>328</v>
       </c>
-      <c r="G44" t="s">
-        <v>329</v>
-      </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N44" t="str">
         <f>+sources!E21</f>
@@ -3558,13 +3563,13 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3573,43 +3578,43 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N45" t="str">
         <f>+sources!E22</f>
-        <v>https://bank.gov.ua/files/fsi_table_1_e.xlsx</v>
+        <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3618,43 +3623,43 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N46" t="str">
         <f>+sources!E22</f>
-        <v>https://bank.gov.ua/files/fsi_table_1_e.xlsx</v>
+        <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3663,28 +3668,28 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J47" t="s">
+        <v>340</v>
+      </c>
+      <c r="K47" t="s">
+        <v>136</v>
+      </c>
+      <c r="L47" t="s">
         <v>341</v>
       </c>
-      <c r="K47" t="s">
-        <v>137</v>
-      </c>
-      <c r="L47" t="s">
-        <v>342</v>
-      </c>
       <c r="M47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N47" t="str">
         <f>+sources!E25</f>
@@ -3693,13 +3698,13 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3708,22 +3713,22 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
+        <v>300</v>
+      </c>
+      <c r="G48" t="s">
         <v>301</v>
       </c>
-      <c r="G48" t="s">
-        <v>302</v>
-      </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N48" t="str">
         <f>+sources!E23</f>
@@ -3732,13 +3737,13 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3747,36 +3752,36 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L49" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M49" t="s">
+        <v>276</v>
+      </c>
+      <c r="N49" t="s">
         <v>277</v>
-      </c>
-      <c r="N49" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3785,36 +3790,36 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G50" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L50" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M50" t="s">
+        <v>276</v>
+      </c>
+      <c r="N50" t="s">
         <v>277</v>
-      </c>
-      <c r="N50" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3823,36 +3828,36 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M51" t="s">
+        <v>276</v>
+      </c>
+      <c r="N51" t="s">
         <v>277</v>
-      </c>
-      <c r="N51" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3861,19 +3866,19 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L52" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M52" t="s">
         <v>16</v>
@@ -3885,13 +3890,13 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3900,19 +3905,19 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
+        <v>332</v>
+      </c>
+      <c r="G53" t="s">
+        <v>297</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
         <v>333</v>
       </c>
-      <c r="G53" t="s">
-        <v>298</v>
-      </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>334</v>
-      </c>
       <c r="L53" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M53" t="s">
         <v>16</v>
@@ -3924,13 +3929,13 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -3939,25 +3944,25 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54" t="s">
+        <v>333</v>
+      </c>
+      <c r="J54" t="s">
+        <v>356</v>
+      </c>
+      <c r="K54" t="s">
         <v>334</v>
       </c>
-      <c r="J54" t="s">
-        <v>357</v>
-      </c>
-      <c r="K54" t="s">
-        <v>335</v>
-      </c>
       <c r="L54" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M54" t="s">
         <v>16</v>
@@ -3969,13 +3974,13 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3984,33 +3989,33 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G55" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M55" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B56" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56" t="s">
         <v>222</v>
-      </c>
-      <c r="C56" t="s">
-        <v>223</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4024,46 +4029,46 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
+        <v>358</v>
+      </c>
+      <c r="B57" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
         <v>359</v>
       </c>
-      <c r="B57" t="s">
-        <v>225</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" t="s">
-        <v>360</v>
-      </c>
       <c r="G57" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K57">
         <v>2021</v>
       </c>
       <c r="L57" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N57" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4087,21 +4092,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" t="s">
-        <v>178</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4112,7 +4117,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>10000000</v>
@@ -4126,7 +4131,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>11000000</v>
@@ -4140,7 +4145,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>11010000</v>
@@ -4154,7 +4159,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>11020000</v>
@@ -4168,7 +4173,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>13000000</v>
@@ -4182,7 +4187,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>13030000</v>
@@ -4196,7 +4201,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9">
         <v>14000000</v>
@@ -4210,7 +4215,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>14020000</v>
@@ -4224,7 +4229,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>14030000</v>
@@ -4238,7 +4243,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>14060000</v>
@@ -4252,7 +4257,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>14070000</v>
@@ -4266,7 +4271,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14">
         <v>18000000</v>
@@ -4280,7 +4285,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>18050000</v>
@@ -4294,7 +4299,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16">
         <v>19000000</v>
@@ -4308,7 +4313,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>19010000</v>
@@ -4322,7 +4327,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>19060000</v>
@@ -4336,7 +4341,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>20000000</v>
@@ -4350,7 +4355,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B20">
         <v>21000000</v>
@@ -4364,7 +4369,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21">
         <v>21010000</v>
@@ -4378,7 +4383,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22">
         <v>21020000</v>
@@ -4392,7 +4397,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23">
         <v>22000000</v>
@@ -4406,7 +4411,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24">
         <v>22010000</v>
@@ -4420,7 +4425,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>22080000</v>
@@ -4434,7 +4439,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26">
         <v>22090000</v>
@@ -4448,7 +4453,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B27">
         <v>24000000</v>
@@ -4462,7 +4467,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>24140000</v>
@@ -4476,7 +4481,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29">
         <v>25000000</v>
@@ -4490,7 +4495,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30">
         <v>30000000</v>
@@ -4504,7 +4509,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B31">
         <v>42000000</v>
@@ -4518,7 +4523,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>50000000</v>
@@ -4547,21 +4552,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" t="s">
-        <v>178</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -4575,7 +4580,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -4589,7 +4594,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -4603,7 +4608,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>400</v>
@@ -4617,7 +4622,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -4631,7 +4636,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7">
         <v>600</v>
@@ -4645,7 +4650,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>700</v>
@@ -4659,7 +4664,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>800</v>
@@ -4673,7 +4678,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10">
         <v>900</v>
@@ -4687,7 +4692,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>1000</v>
@@ -4701,7 +4706,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -4712,7 +4717,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>180</v>
@@ -4726,7 +4731,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -4737,7 +4742,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>2000</v>
@@ -4751,7 +4756,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>2100</v>
@@ -4765,7 +4770,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>2200</v>
@@ -4779,7 +4784,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18">
         <v>2400</v>
@@ -4793,7 +4798,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19">
         <v>2600</v>
@@ -4807,7 +4812,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20">
         <v>2700</v>
@@ -4821,7 +4826,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21">
         <v>2800</v>
@@ -4835,7 +4840,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22">
         <v>3000</v>
@@ -4849,7 +4854,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23">
         <v>3100</v>
@@ -4863,7 +4868,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24">
         <v>3200</v>
@@ -4877,7 +4882,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -4906,21 +4911,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" t="s">
-        <v>178</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4931,7 +4936,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>200000</v>
@@ -4945,7 +4950,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>202000</v>
@@ -4959,7 +4964,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5">
         <v>203000</v>
@@ -4973,7 +4978,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6">
         <v>204000</v>
@@ -4987,7 +4992,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7">
         <v>205000</v>
@@ -5001,7 +5006,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>206000</v>
@@ -5015,7 +5020,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <v>207000</v>
@@ -5029,7 +5034,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10">
         <v>208000</v>
@@ -5043,7 +5048,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>300000</v>
@@ -5057,7 +5062,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B12">
         <v>301000</v>
@@ -5071,7 +5076,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13">
         <v>302000</v>
@@ -5085,7 +5090,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14">
         <v>303000</v>
@@ -5099,7 +5104,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15">
         <v>304000</v>
@@ -5113,7 +5118,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B16">
         <v>305000</v>
@@ -5127,7 +5132,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17">
         <v>307000</v>
@@ -5141,7 +5146,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -5152,7 +5157,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19">
         <v>400000</v>
@@ -5166,7 +5171,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20">
         <v>401000</v>
@@ -5180,7 +5185,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>402000</v>
@@ -5194,7 +5199,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22">
         <v>403000</v>
@@ -5208,7 +5213,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23">
         <v>500000</v>
@@ -5222,7 +5227,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24">
         <v>600000</v>
@@ -5236,7 +5241,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25">
         <v>601000</v>
@@ -5250,7 +5255,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26">
         <v>602000</v>
@@ -5264,7 +5269,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27">
         <v>603000</v>
@@ -5278,7 +5283,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5289,7 +5294,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -5300,7 +5305,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30">
         <v>4000</v>
@@ -5314,7 +5319,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31">
         <v>4110</v>
@@ -5328,7 +5333,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32">
         <v>4120</v>
@@ -5360,15 +5365,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -5376,7 +5381,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -5384,7 +5389,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -5392,7 +5397,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -5400,7 +5405,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -5408,7 +5413,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -5416,7 +5421,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -5424,7 +5429,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -5432,7 +5437,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -5440,7 +5445,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -5448,7 +5453,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -5456,7 +5461,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -5464,7 +5469,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -5487,15 +5492,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -5503,7 +5508,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -5511,7 +5516,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -5519,7 +5524,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -5527,7 +5532,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -5535,7 +5540,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -5561,7 +5566,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -5569,7 +5574,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5577,7 +5582,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5585,7 +5590,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5593,7 +5598,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5601,7 +5606,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5609,7 +5614,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5617,7 +5622,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5625,7 +5630,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5633,7 +5638,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5641,7 +5646,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5649,7 +5654,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5657,7 +5662,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5665,7 +5670,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5673,7 +5678,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5681,7 +5686,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5689,7 +5694,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5697,7 +5702,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5705,7 +5710,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5713,7 +5718,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -5721,7 +5726,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -5729,7 +5734,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -5737,7 +5742,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -5745,7 +5750,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5753,7 +5758,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5761,7 +5766,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -5769,7 +5774,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -5777,7 +5782,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -5785,7 +5790,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5793,7 +5798,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5801,7 +5806,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5809,7 +5814,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5817,7 +5822,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5825,7 +5830,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5833,7 +5838,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5841,7 +5846,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5876,7 +5881,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -5884,7 +5889,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5892,7 +5897,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5900,7 +5905,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5908,7 +5913,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5916,7 +5921,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5924,7 +5929,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5932,7 +5937,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5940,7 +5945,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5948,7 +5953,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5956,7 +5961,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5964,7 +5969,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>

<commit_message>
Updated casualties data and metrics
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukrainedb\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912086A9-38F7-46F2-BAC0-41290418372F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D48FFD-090E-443E-8985-673BF082F239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="371">
   <si>
     <t>source</t>
   </si>
@@ -85,9 +85,6 @@
     <t>https://data.humdata.org/dataset/9b95de1b-d4e9-4c81-b2bb-db35bd9620e8/resource/1730560f-8e9f-4999-bec8-72118ac0ee5f/download/wfp_food_prices_ukr.csv</t>
   </si>
   <si>
-    <t>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/Subject_Dossiers_Topics/Ukraine/Ukraine_Support_Tracker/Ukraine_Support_Tracker.xlsx</t>
-  </si>
-  <si>
     <t>assets/world_bank_reconstruction.xlsx</t>
   </si>
   <si>
@@ -946,9 +943,6 @@
     <t>Non-advanced economies to Total</t>
   </si>
   <si>
-    <t>Civilians killed, confirmed</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -979,9 +973,6 @@
     <t>All</t>
   </si>
   <si>
-    <t>Civilians injured, confirmed</t>
-  </si>
-  <si>
     <t>Internally displaced</t>
   </si>
   <si>
@@ -1099,9 +1090,6 @@
     <t>UAH mn</t>
   </si>
   <si>
-    <t>Civilian deaths, confirmed</t>
-  </si>
-  <si>
     <t>Ukraine</t>
   </si>
   <si>
@@ -1157,6 +1145,30 @@
   </si>
   <si>
     <t>Nonperforming loans net of provisions to capital</t>
+  </si>
+  <si>
+    <t>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</t>
+  </si>
+  <si>
+    <t>tf_civilian_casualties.xlsx</t>
+  </si>
+  <si>
+    <t>Killed</t>
+  </si>
+  <si>
+    <t>Civilians killed since 2022</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>Injured</t>
+  </si>
+  <si>
+    <t>Civilians injured since 2022</t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1586,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1586,16 +1598,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1604,24 +1616,24 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1632,19 +1644,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1652,16 +1664,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -1672,19 +1684,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1692,16 +1704,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -1712,16 +1724,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -1732,16 +1744,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -1752,16 +1764,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -1772,25 +1784,25 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>363</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -1798,71 +1810,71 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1870,25 +1882,25 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1896,19 +1908,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1919,19 +1931,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1942,19 +1954,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1965,19 +1977,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1988,19 +2000,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
         <v>47</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2008,19 +2020,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -2031,19 +2043,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21">
         <v>7</v>
@@ -2057,25 +2069,25 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2083,19 +2095,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -2106,19 +2118,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -2129,19 +2141,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -2152,19 +2164,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" xr:uid="{38DDF94D-136E-4C17-9075-1CDDD155D52D}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{EF5F241D-7A8B-4521-8D86-5DD017C3B9B6}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{B732F35B-FD86-49E5-80C4-3F90C0277558}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{03153242-A8CF-4258-8B5C-E60745E931E9}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{9097FC7E-4B65-4B2E-B670-D1F12245F4D4}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{90554452-6F54-41AB-AA54-4DD7914CB6D5}"/>
-    <hyperlink ref="E25" r:id="rId7" xr:uid="{04E46315-FB46-4EB7-B7CC-4D046B83538C}"/>
-    <hyperlink ref="E24" r:id="rId8" xr:uid="{66BBB48B-BFE8-486A-9602-D62D27CCB40F}"/>
-    <hyperlink ref="E23" r:id="rId9" xr:uid="{373411FC-DB71-4A1B-8AF1-FD47374CEAD6}"/>
-    <hyperlink ref="E20" r:id="rId10" xr:uid="{A0042D51-75FF-4622-92B3-F85244BF1565}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{34D6EFF7-F5DE-4487-A837-7043BEBA7731}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{CB2ABF31-9EE8-4678-BF7F-C2E399CDD67F}"/>
-    <hyperlink ref="E3" r:id="rId13" xr:uid="{8E9E6E0C-1C15-4692-9DB7-C338EBCC85EF}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{EF5F241D-7A8B-4521-8D86-5DD017C3B9B6}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{B732F35B-FD86-49E5-80C4-3F90C0277558}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{03153242-A8CF-4258-8B5C-E60745E931E9}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{9097FC7E-4B65-4B2E-B670-D1F12245F4D4}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{90554452-6F54-41AB-AA54-4DD7914CB6D5}"/>
+    <hyperlink ref="E25" r:id="rId6" xr:uid="{04E46315-FB46-4EB7-B7CC-4D046B83538C}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{66BBB48B-BFE8-486A-9602-D62D27CCB40F}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{373411FC-DB71-4A1B-8AF1-FD47374CEAD6}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{A0042D51-75FF-4622-92B3-F85244BF1565}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{34D6EFF7-F5DE-4487-A837-7043BEBA7731}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{CB2ABF31-9EE8-4678-BF7F-C2E399CDD67F}"/>
+    <hyperlink ref="E3" r:id="rId12" xr:uid="{8E9E6E0C-1C15-4692-9DB7-C338EBCC85EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2186,15 +2197,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2202,7 +2213,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2210,7 +2221,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2218,7 +2229,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2226,7 +2237,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2234,7 +2245,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2242,7 +2253,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2250,7 +2261,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2258,7 +2269,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2266,7 +2277,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2279,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CAA2C0-DB42-4D84-A6A6-1D10E6E62173}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2294,339 +2305,342 @@
     <col min="7" max="12" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>220</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>221</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
         <v>222</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>223</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
         <v>224</v>
       </c>
-      <c r="C3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
         <v>225</v>
       </c>
-      <c r="B4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
         <v>226</v>
       </c>
-      <c r="B5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>227</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
         <v>228</v>
       </c>
-      <c r="C6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
         <v>229</v>
       </c>
-      <c r="B7" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" t="s">
-        <v>222</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
         <v>230</v>
       </c>
-      <c r="B8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
         <v>231</v>
       </c>
-      <c r="B9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9" t="s">
-        <v>222</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
         <v>232</v>
       </c>
-      <c r="B10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
         <v>233</v>
       </c>
-      <c r="B11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
         <v>234</v>
       </c>
-      <c r="B12" t="s">
-        <v>224</v>
-      </c>
-      <c r="C12" t="s">
-        <v>222</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
         <v>235</v>
       </c>
-      <c r="B13" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
         <v>236</v>
       </c>
-      <c r="B14" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" t="s">
-        <v>222</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
         <v>237</v>
       </c>
-      <c r="B15" t="s">
-        <v>224</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" t="s">
-        <v>238</v>
-      </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2640,13 +2654,13 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2660,13 +2674,13 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2680,13 +2694,13 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2700,13 +2714,13 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2720,13 +2734,13 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2740,13 +2754,13 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2760,13 +2774,13 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
         <v>221</v>
-      </c>
-      <c r="C23" t="s">
-        <v>222</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2780,13 +2794,13 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2795,22 +2809,22 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L24" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N24" t="str">
         <f>+sources!E20</f>
@@ -2819,13 +2833,13 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2834,22 +2848,22 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" t="s">
         <v>284</v>
       </c>
-      <c r="G25" t="s">
-        <v>285</v>
-      </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L25" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N25" t="str">
         <f>+sources!E18</f>
@@ -2858,13 +2872,13 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2873,16 +2887,16 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>283</v>
+      </c>
+      <c r="G26" t="s">
         <v>284</v>
       </c>
-      <c r="G26" t="s">
-        <v>285</v>
-      </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N26" t="str">
         <f>+sources!E18</f>
@@ -2891,13 +2905,13 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2909,21 +2923,21 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2932,33 +2946,33 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
+        <v>286</v>
+      </c>
+      <c r="G28" t="s">
         <v>287</v>
       </c>
-      <c r="G28" t="s">
-        <v>288</v>
-      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="M28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2967,33 +2981,33 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="M29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -3002,39 +3016,39 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" t="s">
+        <v>336</v>
+      </c>
+      <c r="J30" t="s">
+        <v>338</v>
+      </c>
+      <c r="K30" t="s">
         <v>339</v>
       </c>
-      <c r="J30" t="s">
-        <v>341</v>
-      </c>
-      <c r="K30" t="s">
-        <v>342</v>
-      </c>
       <c r="M30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -3043,39 +3057,39 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="J31" t="s">
+        <v>338</v>
+      </c>
+      <c r="K31" t="s">
         <v>341</v>
       </c>
-      <c r="K31" t="s">
-        <v>344</v>
-      </c>
       <c r="M31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3084,34 +3098,34 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="M32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N32" t="str">
         <f>+sources!E22</f>
         <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3120,34 +3134,34 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="M33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N33" t="str">
         <f>+sources!E23</f>
         <v>https://bank.gov.ua/files/PInterestRates_e.xls</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3156,37 +3170,37 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L34" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="M34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N34" t="str">
         <f>+sources!E15</f>
         <v>https://bank.gov.ua/files/macro/C_budget_m.xlsx</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3195,40 +3209,40 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="J35" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="K35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N35" t="str">
         <f>+sources!E16</f>
         <v>https://bank.gov.ua/files/macro/C_budget_m.xlsx</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -3237,114 +3251,114 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L36" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="M36" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N36" t="str">
         <f>+sources!E15</f>
         <v>https://bank.gov.ua/files/macro/C_budget_m.xlsx</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
+        <v>254</v>
+      </c>
+      <c r="B37" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>292</v>
+      </c>
+      <c r="G37" t="s">
+        <v>293</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>271</v>
+      </c>
+      <c r="N37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
         <v>255</v>
       </c>
-      <c r="B37" t="s">
-        <v>224</v>
-      </c>
-      <c r="C37" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>293</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>345</v>
+      </c>
+      <c r="G38" t="s">
         <v>294</v>
       </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="M37" t="s">
-        <v>272</v>
-      </c>
-      <c r="N37" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B38" t="s">
-        <v>224</v>
-      </c>
-      <c r="C38" t="s">
-        <v>222</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>349</v>
-      </c>
-      <c r="G38" t="s">
-        <v>295</v>
-      </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J38" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="K38" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="L38" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="M38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N38" t="e">
         <f>+sources!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -3353,34 +3367,34 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N39" t="e">
         <f>+sources!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>364</v>
       </c>
       <c r="B40" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -3389,34 +3403,37 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>296</v>
+        <v>370</v>
       </c>
       <c r="G40" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="M40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N40" t="str">
         <f>+sources!E2</f>
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>257</v>
+        <v>364</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3425,34 +3442,37 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
+        <v>366</v>
+      </c>
+      <c r="G41" t="s">
         <v>307</v>
       </c>
-      <c r="G41" t="s">
-        <v>310</v>
-      </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>307</v>
+        <v>365</v>
       </c>
       <c r="M41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N41" t="str">
         <f>+sources!E2</f>
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="O41" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3461,34 +3481,34 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G42" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N42" t="str">
         <f>+sources!E2</f>
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3497,34 +3517,34 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
+        <v>305</v>
+      </c>
+      <c r="G43" t="s">
         <v>308</v>
       </c>
-      <c r="G43" t="s">
-        <v>311</v>
-      </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="M43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N43" t="str">
         <f>+sources!E2</f>
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3533,43 +3553,43 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G44" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K44" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L44" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M44" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N44" t="str">
         <f>+sources!E21</f>
         <v>https://bank.gov.ua/files/interest_rates_e.xlsx</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3578,43 +3598,43 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G45" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K45" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L45" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M45" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N45" t="str">
         <f>+sources!E22</f>
         <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3623,43 +3643,43 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G46" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K46" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L46" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N46" t="str">
         <f>+sources!E22</f>
         <v>https://bank.gov.ua/files/SDDS/sdds+_fsi_en.xlsx</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3668,43 +3688,43 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G47" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="K47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L47" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N47" t="str">
         <f>+sources!E25</f>
         <v>https://bank.gov.ua/files/SDDS/IREZ_en.xlsx</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3713,22 +3733,22 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L48" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M48" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N48" t="str">
         <f>+sources!E23</f>
@@ -3737,13 +3757,13 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C49" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3752,36 +3772,36 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G49" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L49" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M49" t="s">
+        <v>275</v>
+      </c>
+      <c r="N49" t="s">
         <v>276</v>
-      </c>
-      <c r="N49" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3790,36 +3810,36 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G50" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L50" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M50" t="s">
+        <v>275</v>
+      </c>
+      <c r="N50" t="s">
         <v>276</v>
-      </c>
-      <c r="N50" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3828,36 +3848,36 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G51" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51" t="s">
+        <v>332</v>
+      </c>
+      <c r="L51" t="s">
         <v>335</v>
       </c>
-      <c r="L51" t="s">
-        <v>338</v>
-      </c>
       <c r="M51" t="s">
+        <v>275</v>
+      </c>
+      <c r="N51" t="s">
         <v>276</v>
-      </c>
-      <c r="N51" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3866,37 +3886,37 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G52" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="L52" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N52" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/Subject_Dossiers_Topics/Ukraine/Ukraine_Support_Tracker/Ukraine_Support_Tracker.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3905,37 +3925,37 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G53" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="L53" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N53" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/Subject_Dossiers_Topics/Ukraine/Ukraine_Support_Tracker/Ukraine_Support_Tracker.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -3944,43 +3964,43 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G54" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J54" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K54" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L54" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N54" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/Subject_Dossiers_Topics/Ukraine/Ukraine_Support_Tracker/Ukraine_Support_Tracker.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3989,33 +4009,33 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M55" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B56" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" t="s">
         <v>221</v>
-      </c>
-      <c r="C56" t="s">
-        <v>222</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4029,13 +4049,13 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -4044,31 +4064,31 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G57" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J57" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="K57">
         <v>2021</v>
       </c>
       <c r="L57" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="M57" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="N57" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -4092,21 +4112,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
-        <v>177</v>
-      </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4117,7 +4137,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>10000000</v>
@@ -4131,7 +4151,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>11000000</v>
@@ -4145,7 +4165,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>11010000</v>
@@ -4159,7 +4179,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>11020000</v>
@@ -4173,7 +4193,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7">
         <v>13000000</v>
@@ -4187,7 +4207,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>13030000</v>
@@ -4201,7 +4221,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9">
         <v>14000000</v>
@@ -4215,7 +4235,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>14020000</v>
@@ -4229,7 +4249,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>14030000</v>
@@ -4243,7 +4263,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>14060000</v>
@@ -4257,7 +4277,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>14070000</v>
@@ -4271,7 +4291,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B14">
         <v>18000000</v>
@@ -4285,7 +4305,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15">
         <v>18050000</v>
@@ -4299,7 +4319,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16">
         <v>19000000</v>
@@ -4313,7 +4333,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <v>19010000</v>
@@ -4327,7 +4347,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18">
         <v>19060000</v>
@@ -4341,7 +4361,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19">
         <v>20000000</v>
@@ -4355,7 +4375,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20">
         <v>21000000</v>
@@ -4369,7 +4389,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>21010000</v>
@@ -4383,7 +4403,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22">
         <v>21020000</v>
@@ -4397,7 +4417,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B23">
         <v>22000000</v>
@@ -4411,7 +4431,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24">
         <v>22010000</v>
@@ -4425,7 +4445,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25">
         <v>22080000</v>
@@ -4439,7 +4459,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26">
         <v>22090000</v>
@@ -4453,7 +4473,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B27">
         <v>24000000</v>
@@ -4467,7 +4487,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28">
         <v>24140000</v>
@@ -4481,7 +4501,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29">
         <v>25000000</v>
@@ -4495,7 +4515,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30">
         <v>30000000</v>
@@ -4509,7 +4529,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B31">
         <v>42000000</v>
@@ -4523,7 +4543,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>50000000</v>
@@ -4552,21 +4572,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
-        <v>177</v>
-      </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -4580,7 +4600,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -4594,7 +4614,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -4608,7 +4628,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5">
         <v>400</v>
@@ -4622,7 +4642,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -4636,7 +4656,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7">
         <v>600</v>
@@ -4650,7 +4670,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>700</v>
@@ -4664,7 +4684,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>800</v>
@@ -4678,7 +4698,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>900</v>
@@ -4692,7 +4712,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <v>1000</v>
@@ -4706,7 +4726,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -4717,7 +4737,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>180</v>
@@ -4731,7 +4751,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -4742,7 +4762,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15">
         <v>2000</v>
@@ -4756,7 +4776,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16">
         <v>2100</v>
@@ -4770,7 +4790,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17">
         <v>2200</v>
@@ -4784,7 +4804,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18">
         <v>2400</v>
@@ -4798,7 +4818,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19">
         <v>2600</v>
@@ -4812,7 +4832,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20">
         <v>2700</v>
@@ -4826,7 +4846,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21">
         <v>2800</v>
@@ -4840,7 +4860,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22">
         <v>3000</v>
@@ -4854,7 +4874,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23">
         <v>3100</v>
@@ -4868,7 +4888,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24">
         <v>3200</v>
@@ -4882,7 +4902,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -4911,21 +4931,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
-        <v>177</v>
-      </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4936,7 +4956,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>200000</v>
@@ -4950,7 +4970,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>202000</v>
@@ -4964,7 +4984,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>203000</v>
@@ -4978,7 +4998,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>204000</v>
@@ -4992,7 +5012,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>205000</v>
@@ -5006,7 +5026,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>206000</v>
@@ -5020,7 +5040,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9">
         <v>207000</v>
@@ -5034,7 +5054,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10">
         <v>208000</v>
@@ -5048,7 +5068,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11">
         <v>300000</v>
@@ -5062,7 +5082,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12">
         <v>301000</v>
@@ -5076,7 +5096,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13">
         <v>302000</v>
@@ -5090,7 +5110,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14">
         <v>303000</v>
@@ -5104,7 +5124,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15">
         <v>304000</v>
@@ -5118,7 +5138,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>305000</v>
@@ -5132,7 +5152,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17">
         <v>307000</v>
@@ -5146,7 +5166,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -5157,7 +5177,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>400000</v>
@@ -5171,7 +5191,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20">
         <v>401000</v>
@@ -5185,7 +5205,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21">
         <v>402000</v>
@@ -5199,7 +5219,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22">
         <v>403000</v>
@@ -5213,7 +5233,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23">
         <v>500000</v>
@@ -5227,7 +5247,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24">
         <v>600000</v>
@@ -5241,7 +5261,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25">
         <v>601000</v>
@@ -5255,7 +5275,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26">
         <v>602000</v>
@@ -5269,7 +5289,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27">
         <v>603000</v>
@@ -5283,7 +5303,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5294,7 +5314,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -5305,7 +5325,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30">
         <v>4000</v>
@@ -5319,7 +5339,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B31">
         <v>4110</v>
@@ -5333,7 +5353,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B32">
         <v>4120</v>
@@ -5365,15 +5385,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -5381,7 +5401,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -5389,7 +5409,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -5397,7 +5417,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -5405,7 +5425,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -5413,7 +5433,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -5421,7 +5441,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -5429,7 +5449,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -5437,7 +5457,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -5445,7 +5465,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -5453,7 +5473,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -5461,7 +5481,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -5469,7 +5489,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -5492,15 +5512,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -5508,7 +5528,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -5516,7 +5536,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -5524,7 +5544,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -5532,7 +5552,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -5540,7 +5560,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -5566,15 +5586,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5582,7 +5602,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5590,7 +5610,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5598,7 +5618,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5606,7 +5626,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5614,7 +5634,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5622,7 +5642,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5630,7 +5650,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5638,7 +5658,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5646,7 +5666,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5654,7 +5674,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5662,7 +5682,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5670,7 +5690,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5678,7 +5698,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5686,7 +5706,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5694,7 +5714,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5702,7 +5722,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5710,7 +5730,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5718,7 +5738,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -5726,7 +5746,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -5734,7 +5754,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -5742,7 +5762,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -5750,7 +5770,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5758,7 +5778,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5766,7 +5786,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -5774,7 +5794,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -5782,7 +5802,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -5790,7 +5810,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5798,7 +5818,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5806,7 +5826,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5814,7 +5834,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5822,7 +5842,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5830,7 +5850,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5838,7 +5858,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5846,7 +5866,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5881,15 +5901,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5897,7 +5917,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5905,7 +5925,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5913,7 +5933,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5921,7 +5941,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5929,7 +5949,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5937,7 +5957,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5945,7 +5965,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5953,7 +5973,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5961,7 +5981,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5969,7 +5989,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <v>0</v>

</xml_diff>

<commit_message>
(bugfix): fixed broken links
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukrainedb\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D48FFD-090E-443E-8985-673BF082F239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A128472-53D1-48A9-A6C3-3AA2CD2FBE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -1147,9 +1147,6 @@
     <t>Nonperforming loans net of provisions to capital</t>
   </si>
   <si>
-    <t>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</t>
-  </si>
-  <si>
     <t>tf_civilian_casualties.xlsx</t>
   </si>
   <si>
@@ -1169,6 +1166,9 @@
   </si>
   <si>
     <t>Civilians injured since 2022</t>
+  </si>
+  <si>
+    <t>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/02364ca6-c302-4313-97af-50a7d40eaa21-Ukraine_Support_Tracker_Release_20.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1796,7 +1796,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2292,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CAA2C0-DB42-4D84-A6A6-1D10E6E62173}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -2349,7 +2349,7 @@
         <v>267</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3388,7 +3388,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B40" t="s">
         <v>220</v>
@@ -3403,7 +3403,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G40" t="s">
         <v>307</v>
@@ -3412,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M40" t="s">
         <v>272</v>
@@ -3422,12 +3422,12 @@
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
       <c r="O40" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" t="s">
         <v>220</v>
@@ -3442,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G41" t="s">
         <v>307</v>
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M41" t="s">
         <v>272</v>
@@ -3461,7 +3461,7 @@
         <v>https://proxy.hxlstandard.org/data.csv?tagger-match-all=on&amp;tagger-01-header=total+population%28flash+appeal%29&amp;tagger-01-tag=%23population%2Btotal&amp;tagger-02-header=people+affected%28flash+appeal%29&amp;tagger-02-tag=%23affected%2Btotal&amp;tagger-03-header=people+affected+-+idps&amp;tagger-03-tag=%23affected%2Bidps&amp;tagger-04-header=people+in+need%28flash+appeal%29&amp;tagger-04-tag=%23affected%2Bpin&amp;tagger-05-header=pin+-+idps&amp;tagger-05-tag=%23affected%2Bpin%2Bidps&amp;tagger-06-header=people+targeted%28flash+appeal%29&amp;tagger-06-tag=%23affected%2Bpin%2Bidps&amp;tagger-07-header=people+targeted+-+idps&amp;tagger-07-tag=%23targeted%2Bidps&amp;tagger-11-header=refugees%28unhcr%29&amp;tagger-11-tag=%23affected%2Brefugees&amp;tagger-12-header=civilian+casualities%28unhcr%29+-+killed&amp;tagger-12-tag=%23affected%2Bkilled&amp;tagger-13-header=civilian+casualities%28unhcr%29+-+injured&amp;tagger-13-tag=%23affected%2Binjured&amp;tagger-14-header=date&amp;tagger-14-tag=%23date&amp;tagger-16-header=ukraine+flash+appeal+2022+-+required+%28us%24m%29&amp;tagger-16-tag=%23value%2Bfunding%2Bflash%2Brequired%2Busd&amp;tagger-17-header=ukraine+flash+appeal+2022+-+funded+%28us%24m%29&amp;tagger-17-tag=%23value%2Bfunding%2Bflash%2Bfunded%2Busd&amp;tagger-18-header=ukraine+flash+appeal+2022+-+%25+coverage&amp;tagger-18-tag=%23value%2Bfunding%2Bflash%2Bpct&amp;tagger-19-header=ukraine+humanitarian+response+plan+2022+-+required+%28us%24m%29&amp;tagger-19-tag=%23value%2Bfunding%2Bhrp%2Brequired%2Busd&amp;tagger-20-header=ukraine+humanitarian+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-20-tag=%23value%2Bfunding%2Bhrp%2Bfunded%2Busd&amp;tagger-21-header=ukraine+humanitarian+response+plan+2022+-+%25+coverage&amp;tagger-21-tag=%23value%2Bfunding%2Bhrp%2Bpct&amp;tagger-22-header=ukraine+regional+refugee+response+plan+2022+-+required+%28us%24m%29&amp;tagger-22-tag=%23value%2Bfunding%2Brrrp%2Brequired%2Busd&amp;tagger-23-header=ukraine+regional+refugee+response+plan+2022+-+funded+%28us%24m%29&amp;tagger-23-tag=%23value%2Bfunding%2Brrrp%2Bfunded%2Busd&amp;tagger-24-header=ukraine+regional+refugee+response+plan+2022+-+%25+coverage&amp;tagger-24-tag=%23value%2Bfunding%2Brrrp%2Bpct&amp;tagger-25-header=cerf+-+contributions+%28us%24m%29&amp;tagger-25-tag=%23value%2Bcerf%2Bcontributions&amp;tagger-26-header=cerf+-+allocations+%28us%24m%29&amp;tagger-26-tag=%23value%2Bcerf%2Ballocations&amp;tagger-27-header=ukraine+humanitarian+fund+-+contributions+%28us%24m%29&amp;tagger-27-tag=%23value%2Bfunding%2Buhf%2Bcontributions&amp;tagger-28-header=ukraine+humanitarian+fund+-+allocations+%28us%24m%29&amp;tagger-28-tag=%23value%2Bfunding%2Buhf%2Ballocations&amp;url=https%3A%2F%2Fdocs.google.com%2Fspreadsheets%2Fd%2Fe%2F2PACX-1vQIdedbZz0ehRC0b4fsWiP14R7MdtU1mpmwAkuXUPElSah2AWCURKGALFDuHjvyJUL8vzZAt3R1B5qg%2Fpub%3Foutput%3Dcsv&amp;header-row=2&amp;dest=data_view&amp;_gl=1*15fuvam*_ga*MTEzODI5NDY2My4xNjY3NDAzMjYw*_ga_E60ZNX2F68*MTY2NzQwMzI2MC4xLjEuMTY2NzQwMzQyMi4xNy4wLjA.</v>
       </c>
       <c r="O41" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="N52" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/02364ca6-c302-4313-97af-50a7d40eaa21-Ukraine_Support_Tracker_Release_20.xlsx</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="N53" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/02364ca6-c302-4313-97af-50a7d40eaa21-Ukraine_Support_Tracker_Release_20.xlsx</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="N54" t="str">
         <f>+sources!E10</f>
-        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/97d5c1a6-7ed8-4576-b666-ee91f20ae58f-Ukraine_Support_Tracker_Release_18.xlsx</v>
+        <v>https://www.ifw-kiel.de/fileadmin/Dateiverwaltung/IfW-Publications/fis-import/02364ca6-c302-4313-97af-50a7d40eaa21-Ukraine_Support_Tracker_Release_20.xlsx</v>
       </c>
     </row>
     <row r="55" spans="1:14">

</xml_diff>